<commit_message>
Chargement des TI pour la semaine
</commit_message>
<xml_diff>
--- a/Excel/TI/Mon_TI_2024_03_05.xlsx
+++ b/Excel/TI/Mon_TI_2024_03_05.xlsx
@@ -653,7 +653,7 @@
         <v>52.1</v>
       </c>
       <c r="I2" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -665,7 +665,7 @@
         <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="N2" t="n">
         <v>56</v>
@@ -774,17 +774,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Donovan Mitchell</t>
+          <t>Jalen Brunson</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Day-To-Day</t>
+          <t>Questionable</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -794,47 +794,45 @@
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
-        <v>38.4</v>
+        <v>30.8</v>
       </c>
       <c r="G3" t="n">
-        <v>41.1</v>
+        <v>39.6</v>
       </c>
       <c r="H3" t="n">
-        <v>39.9</v>
+        <v>38.2</v>
       </c>
       <c r="I3" t="n">
         <v>9</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M3" t="n">
-        <v>6</v>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P3" t="n">
-        <v>21</v>
+        <v>5</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-1</v>
+      </c>
+      <c r="O3" t="n">
+        <v>32</v>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Q3" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="R3" t="n">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="S3" t="inlineStr">
         <is>
@@ -843,7 +841,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -852,7 +850,7 @@
         </is>
       </c>
       <c r="V3" t="n">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="W3" t="inlineStr">
         <is>
@@ -860,7 +858,7 @@
         </is>
       </c>
       <c r="X3" t="n">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
@@ -874,12 +872,12 @@
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>ORL</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
@@ -889,7 +887,7 @@
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
@@ -899,17 +897,17 @@
       </c>
       <c r="AF3" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="AI3" t="inlineStr">
@@ -918,7 +916,7 @@
         </is>
       </c>
       <c r="AJ3" t="n">
-        <v>4</v>
+        <v>1.6</v>
       </c>
       <c r="AK3" t="inlineStr"/>
       <c r="AL3" t="inlineStr"/>
@@ -926,122 +924,118 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jalen Brunson</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Day-To-Day</t>
-        </is>
-      </c>
+          <t>Zion Williamson</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
-        <v>30.8</v>
+        <v>29.8</v>
       </c>
       <c r="G4" t="n">
-        <v>39.6</v>
+        <v>37.1</v>
       </c>
       <c r="H4" t="n">
-        <v>38.2</v>
+        <v>36.2</v>
       </c>
       <c r="I4" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J4" t="n">
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L4" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N4" t="n">
-        <v>-1</v>
+        <v>13</v>
       </c>
       <c r="O4" t="n">
+        <v>28</v>
+      </c>
+      <c r="P4" t="n">
+        <v>31</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>40</v>
+      </c>
+      <c r="R4" t="n">
+        <v>37</v>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="V4" t="n">
         <v>32</v>
       </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q4" t="n">
-        <v>46</v>
-      </c>
-      <c r="R4" t="n">
-        <v>47</v>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
         <is>
           <t>ATL</t>
         </is>
       </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="V4" t="n">
-        <v>30</v>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="X4" t="n">
-        <v>42</v>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>ORL</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>PHI</t>
-        </is>
-      </c>
       <c r="AE4" t="inlineStr">
         <is>
           <t>vs</t>
@@ -1049,26 +1043,26 @@
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ4" t="n">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="AK4" t="inlineStr"/>
       <c r="AL4" t="inlineStr"/>
@@ -1076,77 +1070,87 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Zion Williamson</t>
+          <t>LaMelo Ball</t>
         </is>
       </c>
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
-        <v>29.8</v>
+        <v>30</v>
       </c>
       <c r="G5" t="n">
-        <v>37.1</v>
+        <v>36.3</v>
       </c>
       <c r="H5" t="n">
-        <v>36.2</v>
+        <v>33.5</v>
       </c>
       <c r="I5" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
-      </c>
-      <c r="N5" t="n">
-        <v>13</v>
-      </c>
-      <c r="O5" t="n">
-        <v>28</v>
-      </c>
-      <c r="P5" t="n">
-        <v>31</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>40</v>
-      </c>
-      <c r="R5" t="n">
-        <v>37</v>
+        <v>0</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>ORL</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="V5" t="n">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="W5" t="inlineStr">
         <is>
@@ -1175,46 +1179,46 @@
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ5" t="n">
-        <v>0</v>
+        <v>2.8</v>
       </c>
       <c r="AK5" t="inlineStr"/>
       <c r="AL5" t="inlineStr"/>
@@ -1222,97 +1226,91 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CHA</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>LaMelo Ball</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr"/>
+          <t>Kristaps Porzingis</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Questionable</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="G6" t="n">
         <v>36.3</v>
       </c>
       <c r="H6" t="n">
-        <v>33.5</v>
+        <v>33.4</v>
       </c>
       <c r="I6" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N6" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+      <c r="O6" t="n">
+        <v>39</v>
+      </c>
+      <c r="P6" t="n">
+        <v>47</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>40</v>
+      </c>
+      <c r="R6" t="n">
+        <v>13</v>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="V6" t="n">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="X6" t="n">
+        <v>35</v>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
@@ -1331,17 +1329,17 @@
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
@@ -1351,7 +1349,7 @@
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
@@ -1361,16 +1359,16 @@
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>UTA</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ6" t="n">
-        <v>2.8</v>
+        <v>-0.4</v>
       </c>
       <c r="AK6" t="inlineStr"/>
       <c r="AL6" t="inlineStr"/>
@@ -1378,65 +1376,61 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Kristaps Porzingis</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Day-To-Day</t>
-        </is>
-      </c>
+          <t>Brandon Ingram</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr"/>
       <c r="D7" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
-        <v>33</v>
+        <v>38.8</v>
       </c>
       <c r="G7" t="n">
-        <v>36.3</v>
+        <v>35.6</v>
       </c>
       <c r="H7" t="n">
-        <v>33.4</v>
+        <v>33.2</v>
       </c>
       <c r="I7" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M7" t="n">
-        <v>6</v>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>4</v>
+      </c>
+      <c r="N7" t="n">
+        <v>57</v>
       </c>
       <c r="O7" t="n">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="P7" t="n">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="Q7" t="n">
-        <v>40</v>
-      </c>
-      <c r="R7" t="n">
-        <v>13</v>
+        <v>26</v>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
@@ -1445,73 +1439,75 @@
       </c>
       <c r="T7" t="inlineStr">
         <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="V7" t="n">
+        <v>74</v>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>PHI</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>ATL</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
           <t>CLE</t>
         </is>
       </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="V7" t="n">
-        <v>25</v>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="X7" t="n">
-        <v>35</v>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>DEN</t>
-        </is>
-      </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AD7" t="inlineStr">
-        <is>
-          <t>PHX</t>
-        </is>
-      </c>
-      <c r="AE7" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AF7" t="inlineStr">
-        <is>
-          <t>POR</t>
-        </is>
-      </c>
       <c r="AG7" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>UTA</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr">
@@ -1520,7 +1516,7 @@
         </is>
       </c>
       <c r="AJ7" t="n">
-        <v>-0.4</v>
+        <v>-2.9</v>
       </c>
       <c r="AK7" t="inlineStr"/>
       <c r="AL7" t="inlineStr"/>
@@ -1528,70 +1524,68 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Brandon Ingram</t>
+          <t>Bam Adebayo</t>
         </is>
       </c>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
-        <v>38.8</v>
+        <v>36.8</v>
       </c>
       <c r="G8" t="n">
-        <v>35.6</v>
+        <v>35.1</v>
       </c>
       <c r="H8" t="n">
-        <v>33.2</v>
+        <v>38.1</v>
       </c>
       <c r="I8" t="n">
         <v>10</v>
       </c>
       <c r="J8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M8" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="N8" t="n">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="O8" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="P8" t="n">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="Q8" t="n">
-        <v>26</v>
-      </c>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>51</v>
+      </c>
+      <c r="R8" t="n">
+        <v>37</v>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="U8" t="inlineStr">
@@ -1600,7 +1594,7 @@
         </is>
       </c>
       <c r="V8" t="n">
-        <v>74</v>
+        <v>40</v>
       </c>
       <c r="W8" t="inlineStr">
         <is>
@@ -1629,7 +1623,7 @@
       </c>
       <c r="AB8" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>DAL</t>
         </is>
       </c>
       <c r="AC8" t="inlineStr">
@@ -1639,7 +1633,7 @@
       </c>
       <c r="AD8" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr">
@@ -1649,7 +1643,7 @@
       </c>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr">
@@ -1659,16 +1653,16 @@
       </c>
       <c r="AH8" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="AI8" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ8" t="n">
-        <v>-2.9</v>
+        <v>-1</v>
       </c>
       <c r="AK8" t="inlineStr"/>
       <c r="AL8" t="inlineStr"/>
@@ -1676,68 +1670,68 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Bam Adebayo</t>
+          <t>Tyrese Maxey</t>
         </is>
       </c>
       <c r="C9" t="inlineStr"/>
       <c r="D9" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
-        <v>36.8</v>
+        <v>37.8</v>
       </c>
       <c r="G9" t="n">
-        <v>35.1</v>
+        <v>34.7</v>
       </c>
       <c r="H9" t="n">
-        <v>38.1</v>
+        <v>35.9</v>
       </c>
       <c r="I9" t="n">
         <v>11</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" t="n">
         <v>1</v>
       </c>
       <c r="L9" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M9" t="n">
         <v>5</v>
       </c>
       <c r="N9" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="O9" t="n">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="P9" t="n">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="Q9" t="n">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="R9" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="S9" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="U9" t="inlineStr">
@@ -1746,17 +1740,15 @@
         </is>
       </c>
       <c r="V9" t="n">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="W9" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="X9" t="n">
+        <v>36</v>
       </c>
       <c r="Y9" t="inlineStr">
         <is>
@@ -1770,51 +1762,51 @@
       </c>
       <c r="AA9" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AB9" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AC9" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AD9" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="AE9" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF9" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="AG9" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AH9" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="AI9" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ9" t="n">
-        <v>-1</v>
+        <v>0.4</v>
       </c>
       <c r="AK9" t="inlineStr"/>
       <c r="AL9" t="inlineStr"/>
@@ -1822,12 +1814,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Tyrese Maxey</t>
+          <t>Dejounte Murray</t>
         </is>
       </c>
       <c r="C10" t="inlineStr"/>
@@ -1838,43 +1830,43 @@
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
-        <v>37.8</v>
+        <v>36.4</v>
       </c>
       <c r="G10" t="n">
-        <v>34.7</v>
+        <v>33.9</v>
       </c>
       <c r="H10" t="n">
-        <v>35.9</v>
+        <v>30.9</v>
       </c>
       <c r="I10" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J10" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" t="n">
+        <v>3</v>
+      </c>
+      <c r="L10" t="n">
         <v>1</v>
       </c>
-      <c r="L10" t="n">
-        <v>3</v>
-      </c>
       <c r="M10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N10" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O10" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="P10" t="n">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="Q10" t="n">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="R10" t="n">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="S10" t="inlineStr">
         <is>
@@ -1883,7 +1875,7 @@
       </c>
       <c r="T10" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="U10" t="inlineStr">
@@ -1892,15 +1884,15 @@
         </is>
       </c>
       <c r="V10" t="n">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="W10" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="X10" t="n">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="Y10" t="inlineStr">
         <is>
@@ -1919,29 +1911,29 @@
       </c>
       <c r="AB10" t="inlineStr">
         <is>
+          <t>CLE</t>
+        </is>
+      </c>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AD10" t="inlineStr">
+        <is>
           <t>MEM</t>
         </is>
       </c>
-      <c r="AC10" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AD10" t="inlineStr">
+      <c r="AE10" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AF10" t="inlineStr">
         <is>
           <t>NOP</t>
         </is>
       </c>
-      <c r="AE10" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AF10" t="inlineStr">
-        <is>
-          <t>NYK</t>
-        </is>
-      </c>
       <c r="AG10" t="inlineStr">
         <is>
           <t>@</t>
@@ -1949,7 +1941,7 @@
       </c>
       <c r="AH10" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="AI10" t="inlineStr">
@@ -1958,7 +1950,7 @@
         </is>
       </c>
       <c r="AJ10" t="n">
-        <v>0.4</v>
+        <v>-1.3</v>
       </c>
       <c r="AK10" t="inlineStr"/>
       <c r="AL10" t="inlineStr"/>
@@ -1966,32 +1958,32 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Dejounte Murray</t>
+          <t>Evan Mobley</t>
         </is>
       </c>
       <c r="C11" t="inlineStr"/>
       <c r="D11" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>C</t>
         </is>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>36.4</v>
+        <v>38.6</v>
       </c>
       <c r="G11" t="n">
-        <v>33.9</v>
+        <v>33.8</v>
       </c>
       <c r="H11" t="n">
-        <v>30.9</v>
+        <v>32.8</v>
       </c>
       <c r="I11" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="J11" t="n">
         <v>1</v>
@@ -2000,51 +1992,55 @@
         <v>3</v>
       </c>
       <c r="L11" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M11" t="n">
         <v>4</v>
       </c>
       <c r="N11" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O11" t="n">
+        <v>54</v>
+      </c>
+      <c r="P11" t="n">
+        <v>43</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>26</v>
+      </c>
+      <c r="R11" t="n">
         <v>40</v>
       </c>
-      <c r="P11" t="n">
-        <v>23</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>45</v>
-      </c>
-      <c r="R11" t="n">
-        <v>43</v>
-      </c>
       <c r="S11" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T11" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="V11" t="n">
-        <v>16</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="W11" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="X11" t="n">
-        <v>29</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Y11" t="inlineStr">
         <is>
@@ -2058,22 +2054,22 @@
       </c>
       <c r="AA11" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AB11" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="AC11" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AD11" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AE11" t="inlineStr">
@@ -2083,26 +2079,26 @@
       </c>
       <c r="AF11" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="AG11" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AH11" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="AI11" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ11" t="n">
-        <v>-1.3</v>
+        <v>-1.4</v>
       </c>
       <c r="AK11" t="inlineStr"/>
       <c r="AL11" t="inlineStr"/>
@@ -2115,7 +2111,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Evan Mobley</t>
+          <t>Jarrett Allen</t>
         </is>
       </c>
       <c r="C12" t="inlineStr"/>
@@ -2126,13 +2122,13 @@
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>38.6</v>
+        <v>32</v>
       </c>
       <c r="G12" t="n">
-        <v>33.8</v>
+        <v>33.6</v>
       </c>
       <c r="H12" t="n">
-        <v>32.8</v>
+        <v>33.6</v>
       </c>
       <c r="I12" t="n">
         <v>13</v>
@@ -2141,28 +2137,28 @@
         <v>1</v>
       </c>
       <c r="K12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L12" t="n">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="M12" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N12" t="n">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="O12" t="n">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="P12" t="n">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="Q12" t="n">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="R12" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="S12" t="inlineStr">
         <is>
@@ -2176,23 +2172,19 @@
       </c>
       <c r="U12" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="V12" t="n">
+        <v>19</v>
       </c>
       <c r="W12" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X12" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="X12" t="n">
+        <v>29</v>
       </c>
       <c r="Y12" t="inlineStr">
         <is>
@@ -2250,7 +2242,7 @@
         </is>
       </c>
       <c r="AJ12" t="n">
-        <v>-1.4</v>
+        <v>1.5</v>
       </c>
       <c r="AK12" t="inlineStr"/>
       <c r="AL12" t="inlineStr"/>
@@ -2258,12 +2250,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Jarrett Allen</t>
+          <t>Jalen Duren</t>
         </is>
       </c>
       <c r="C13" t="inlineStr"/>
@@ -2274,52 +2266,52 @@
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G13" t="n">
-        <v>33.6</v>
+        <v>32.7</v>
       </c>
       <c r="H13" t="n">
-        <v>33.6</v>
+        <v>31.3</v>
       </c>
       <c r="I13" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" t="n">
         <v>2</v>
       </c>
       <c r="L13" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="M13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N13" t="n">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="O13" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="P13" t="n">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="Q13" t="n">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="R13" t="n">
         <v>41</v>
       </c>
       <c r="S13" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T13" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="U13" t="inlineStr">
@@ -2328,15 +2320,17 @@
         </is>
       </c>
       <c r="V13" t="n">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="X13" t="n">
-        <v>29</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Y13" t="inlineStr">
         <is>
@@ -2350,12 +2344,12 @@
       </c>
       <c r="AA13" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AB13" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="AC13" t="inlineStr">
@@ -2365,7 +2359,7 @@
       </c>
       <c r="AD13" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>DAL</t>
         </is>
       </c>
       <c r="AE13" t="inlineStr">
@@ -2375,7 +2369,7 @@
       </c>
       <c r="AF13" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="AG13" t="inlineStr">
@@ -2385,16 +2379,16 @@
       </c>
       <c r="AH13" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="AI13" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ13" t="n">
-        <v>1.5</v>
+        <v>0.1</v>
       </c>
       <c r="AK13" t="inlineStr"/>
       <c r="AL13" t="inlineStr"/>
@@ -2402,18 +2396,18 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Jalen Duren</t>
+          <t>Pascal Siakam</t>
         </is>
       </c>
       <c r="C14" t="inlineStr"/>
       <c r="D14" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E14" t="inlineStr"/>
@@ -2424,13 +2418,13 @@
         <v>32.7</v>
       </c>
       <c r="H14" t="n">
-        <v>31.3</v>
+        <v>34.4</v>
       </c>
       <c r="I14" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K14" t="n">
         <v>3</v>
@@ -2442,19 +2436,19 @@
         <v>3</v>
       </c>
       <c r="N14" t="n">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="O14" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="P14" t="n">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="Q14" t="n">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="R14" t="n">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="S14" t="inlineStr">
         <is>
@@ -2463,26 +2457,24 @@
       </c>
       <c r="T14" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>DAL</t>
         </is>
       </c>
       <c r="U14" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="V14" t="n">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="W14" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X14" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="X14" t="n">
+        <v>43</v>
       </c>
       <c r="Y14" t="inlineStr">
         <is>
@@ -2501,27 +2493,27 @@
       </c>
       <c r="AB14" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AC14" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AD14" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>ORL</t>
         </is>
       </c>
       <c r="AE14" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF14" t="inlineStr">
         <is>
-          <t>CHA</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="AG14" t="inlineStr">
@@ -2531,7 +2523,7 @@
       </c>
       <c r="AH14" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>CHI</t>
         </is>
       </c>
       <c r="AI14" t="inlineStr">
@@ -2540,7 +2532,7 @@
         </is>
       </c>
       <c r="AJ14" t="n">
-        <v>0.1</v>
+        <v>-1.7</v>
       </c>
       <c r="AK14" t="inlineStr"/>
       <c r="AL14" t="inlineStr"/>
@@ -2548,32 +2540,36 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Pascal Siakam</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr"/>
+          <t>Jaylen Brown</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Questionable</t>
+        </is>
+      </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="G15" t="n">
-        <v>32.7</v>
+        <v>31.9</v>
       </c>
       <c r="H15" t="n">
-        <v>34.4</v>
+        <v>31.1</v>
       </c>
       <c r="I15" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="J15" t="n">
         <v>1</v>
@@ -2582,51 +2578,51 @@
         <v>3</v>
       </c>
       <c r="L15" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M15" t="n">
         <v>4</v>
       </c>
       <c r="N15" t="n">
+        <v>40</v>
+      </c>
+      <c r="O15" t="n">
+        <v>40</v>
+      </c>
+      <c r="P15" t="n">
+        <v>49</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>40</v>
+      </c>
+      <c r="R15" t="n">
+        <v>36</v>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>CLE</t>
+        </is>
+      </c>
+      <c r="U15" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="V15" t="n">
         <v>31</v>
       </c>
-      <c r="O15" t="n">
-        <v>15</v>
-      </c>
-      <c r="P15" t="n">
-        <v>43</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>42</v>
-      </c>
-      <c r="R15" t="n">
-        <v>24</v>
-      </c>
-      <c r="S15" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="T15" t="inlineStr">
-        <is>
-          <t>DAL</t>
-        </is>
-      </c>
-      <c r="U15" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="V15" t="n">
-        <v>24</v>
-      </c>
       <c r="W15" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="X15" t="n">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="Y15" t="inlineStr">
         <is>
@@ -2640,12 +2636,12 @@
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="AC15" t="inlineStr">
@@ -2655,7 +2651,7 @@
       </c>
       <c r="AD15" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="AE15" t="inlineStr">
@@ -2665,17 +2661,17 @@
       </c>
       <c r="AF15" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="AG15" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AH15" t="inlineStr">
         <is>
-          <t>CHI</t>
+          <t>UTA</t>
         </is>
       </c>
       <c r="AI15" t="inlineStr">
@@ -2684,7 +2680,7 @@
         </is>
       </c>
       <c r="AJ15" t="n">
-        <v>-1.7</v>
+        <v>-2.4</v>
       </c>
       <c r="AK15" t="inlineStr"/>
       <c r="AL15" t="inlineStr"/>
@@ -2692,85 +2688,87 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>ORL</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Jaylen Brown</t>
+          <t>Franz Wagner</t>
         </is>
       </c>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
-        <v>41</v>
+        <v>24.6</v>
       </c>
       <c r="G16" t="n">
-        <v>31.9</v>
+        <v>30.9</v>
       </c>
       <c r="H16" t="n">
-        <v>31.1</v>
+        <v>30.1</v>
       </c>
       <c r="I16" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="J16" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L16" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="N16" t="n">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="O16" t="n">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="P16" t="n">
+        <v>37</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>28</v>
+      </c>
+      <c r="R16" t="n">
+        <v>15</v>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>CHA</t>
+        </is>
+      </c>
+      <c r="U16" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="V16" t="n">
         <v>49</v>
       </c>
-      <c r="Q16" t="n">
-        <v>40</v>
-      </c>
-      <c r="R16" t="n">
-        <v>36</v>
-      </c>
-      <c r="S16" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="T16" t="inlineStr">
-        <is>
-          <t>CLE</t>
-        </is>
-      </c>
-      <c r="U16" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="V16" t="n">
-        <v>31</v>
-      </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="X16" t="n">
-        <v>34</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Y16" t="inlineStr">
         <is>
@@ -2789,7 +2787,7 @@
       </c>
       <c r="AB16" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="AC16" t="inlineStr">
@@ -2799,27 +2797,27 @@
       </c>
       <c r="AD16" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="AE16" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF16" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="AG16" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AH16" t="inlineStr">
         <is>
-          <t>UTA</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="AI16" t="inlineStr">
@@ -2828,7 +2826,7 @@
         </is>
       </c>
       <c r="AJ16" t="n">
-        <v>-2.4</v>
+        <v>-2.8</v>
       </c>
       <c r="AK16" t="inlineStr"/>
       <c r="AL16" t="inlineStr"/>
@@ -2836,12 +2834,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Franz Wagner</t>
+          <t>RJ Barrett</t>
         </is>
       </c>
       <c r="C17" t="inlineStr"/>
@@ -2852,61 +2850,63 @@
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
-        <v>24.6</v>
+        <v>31</v>
       </c>
       <c r="G17" t="n">
-        <v>30.9</v>
+        <v>30.7</v>
       </c>
       <c r="H17" t="n">
-        <v>30.1</v>
+        <v>27.2</v>
       </c>
       <c r="I17" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="J17" t="n">
         <v>3</v>
       </c>
       <c r="K17" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="M17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="N17" t="n">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="O17" t="n">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="P17" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="Q17" t="n">
-        <v>28</v>
-      </c>
-      <c r="R17" t="n">
-        <v>15</v>
+        <v>33</v>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S17" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T17" t="inlineStr">
         <is>
-          <t>CHA</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="U17" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="V17" t="n">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="W17" t="inlineStr">
         <is>
@@ -2935,7 +2935,7 @@
       </c>
       <c r="AB17" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="AC17" t="inlineStr">
@@ -2945,36 +2945,36 @@
       </c>
       <c r="AD17" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="AE17" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF17" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="AG17" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AH17" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="AI17" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ17" t="n">
-        <v>-2.8</v>
+        <v>1</v>
       </c>
       <c r="AK17" t="inlineStr"/>
       <c r="AL17" t="inlineStr"/>
@@ -2982,80 +2982,78 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>RJ Barrett</t>
+          <t>Cade Cunningham</t>
         </is>
       </c>
       <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G18" t="n">
-        <v>30.7</v>
+        <v>30.1</v>
       </c>
       <c r="H18" t="n">
-        <v>27.2</v>
+        <v>31.4</v>
       </c>
       <c r="I18" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>2</v>
+      </c>
+      <c r="L18" t="n">
+        <v>4</v>
+      </c>
+      <c r="M18" t="n">
         <v>3</v>
       </c>
-      <c r="K18" t="n">
-        <v>0</v>
-      </c>
-      <c r="L18" t="n">
-        <v>7</v>
-      </c>
-      <c r="M18" t="n">
-        <v>1</v>
-      </c>
       <c r="N18" t="n">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="O18" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P18" t="n">
+        <v>43</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>52</v>
+      </c>
+      <c r="R18" t="n">
+        <v>38</v>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>MIA</t>
+        </is>
+      </c>
+      <c r="U18" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="V18" t="n">
         <v>39</v>
       </c>
-      <c r="Q18" t="n">
-        <v>33</v>
-      </c>
-      <c r="R18" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="S18" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="T18" t="inlineStr">
-        <is>
-          <t>NOP</t>
-        </is>
-      </c>
-      <c r="U18" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="V18" t="n">
-        <v>17</v>
-      </c>
       <c r="W18" t="inlineStr">
         <is>
           <t>-</t>
@@ -3078,51 +3076,51 @@
       </c>
       <c r="AA18" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AB18" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="AC18" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AD18" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>DAL</t>
         </is>
       </c>
       <c r="AE18" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF18" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="AG18" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AH18" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="AI18" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ18" t="n">
-        <v>1</v>
+        <v>-1.6</v>
       </c>
       <c r="AK18" t="inlineStr"/>
       <c r="AL18" t="inlineStr"/>
@@ -3130,12 +3128,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Cade Cunningham</t>
+          <t>Jamal Murray</t>
         </is>
       </c>
       <c r="C19" t="inlineStr"/>
@@ -3146,129 +3144,133 @@
       </c>
       <c r="E19" t="inlineStr"/>
       <c r="F19" t="n">
-        <v>35</v>
+        <v>33.8</v>
       </c>
       <c r="G19" t="n">
-        <v>30.1</v>
+        <v>29.4</v>
       </c>
       <c r="H19" t="n">
-        <v>31.4</v>
+        <v>30.8</v>
       </c>
       <c r="I19" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J19" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K19" t="n">
+        <v>0</v>
+      </c>
+      <c r="L19" t="n">
         <v>2</v>
-      </c>
-      <c r="L19" t="n">
-        <v>5</v>
       </c>
       <c r="M19" t="n">
         <v>3</v>
       </c>
       <c r="N19" t="n">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="O19" t="n">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="P19" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="Q19" t="n">
-        <v>52</v>
-      </c>
-      <c r="R19" t="n">
-        <v>38</v>
+        <v>40</v>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S19" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T19" t="inlineStr">
         <is>
+          <t>PHX</t>
+        </is>
+      </c>
+      <c r="U19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="AA19" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AB19" t="inlineStr">
+        <is>
+          <t>BOS</t>
+        </is>
+      </c>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AD19" t="inlineStr">
+        <is>
+          <t>UTA</t>
+        </is>
+      </c>
+      <c r="AE19" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AF19" t="inlineStr">
+        <is>
+          <t>TOR</t>
+        </is>
+      </c>
+      <c r="AG19" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AH19" t="inlineStr">
+        <is>
           <t>MIA</t>
         </is>
       </c>
-      <c r="U19" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="V19" t="n">
-        <v>39</v>
-      </c>
-      <c r="W19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Y19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="AA19" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AB19" t="inlineStr">
-        <is>
-          <t>BKN</t>
-        </is>
-      </c>
-      <c r="AC19" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AD19" t="inlineStr">
-        <is>
-          <t>DAL</t>
-        </is>
-      </c>
-      <c r="AE19" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AF19" t="inlineStr">
-        <is>
-          <t>CHA</t>
-        </is>
-      </c>
-      <c r="AG19" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AH19" t="inlineStr">
-        <is>
-          <t>TOR</t>
-        </is>
-      </c>
       <c r="AI19" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ19" t="n">
-        <v>-1.6</v>
+        <v>0</v>
       </c>
       <c r="AK19" t="inlineStr"/>
       <c r="AL19" t="inlineStr"/>
@@ -3276,81 +3278,77 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Jamal Murray</t>
+          <t>Tobias Harris</t>
         </is>
       </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E20" t="inlineStr"/>
       <c r="F20" t="n">
-        <v>33.8</v>
+        <v>28.8</v>
       </c>
       <c r="G20" t="n">
-        <v>29.4</v>
+        <v>27.7</v>
       </c>
       <c r="H20" t="n">
-        <v>30.8</v>
+        <v>28.7</v>
       </c>
       <c r="I20" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J20" t="n">
+        <v>4</v>
+      </c>
+      <c r="K20" t="n">
+        <v>2</v>
+      </c>
+      <c r="L20" t="n">
         <v>3</v>
       </c>
-      <c r="K20" t="n">
-        <v>0</v>
-      </c>
-      <c r="L20" t="n">
-        <v>2</v>
-      </c>
       <c r="M20" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="N20" t="n">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="O20" t="n">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="P20" t="n">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="Q20" t="n">
-        <v>40</v>
-      </c>
-      <c r="R20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>14</v>
+      </c>
+      <c r="R20" t="n">
+        <v>29</v>
       </c>
       <c r="S20" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T20" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="U20" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V20" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="V20" t="n">
+        <v>11</v>
       </c>
       <c r="W20" t="inlineStr">
         <is>
@@ -3379,7 +3377,7 @@
       </c>
       <c r="AB20" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AC20" t="inlineStr">
@@ -3389,17 +3387,17 @@
       </c>
       <c r="AD20" t="inlineStr">
         <is>
-          <t>UTA</t>
+          <t>NOP</t>
         </is>
       </c>
       <c r="AE20" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF20" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="AG20" t="inlineStr">
@@ -3409,16 +3407,16 @@
       </c>
       <c r="AH20" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="AI20" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ20" t="n">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="AK20" t="inlineStr"/>
       <c r="AL20" t="inlineStr"/>
@@ -3426,59 +3424,65 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Tobias Harris</t>
+          <t>Bradley Beal</t>
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
-        <v>28.8</v>
+        <v>26</v>
       </c>
       <c r="G21" t="n">
-        <v>27.7</v>
+        <v>26.9</v>
       </c>
       <c r="H21" t="n">
-        <v>28.7</v>
+        <v>26.2</v>
       </c>
       <c r="I21" t="n">
+        <v>6</v>
+      </c>
+      <c r="J21" t="n">
+        <v>2</v>
+      </c>
+      <c r="K21" t="n">
+        <v>1</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1</v>
+      </c>
+      <c r="M21" t="n">
+        <v>2</v>
+      </c>
+      <c r="N21" t="n">
+        <v>48</v>
+      </c>
+      <c r="O21" t="n">
         <v>10</v>
       </c>
-      <c r="J21" t="n">
-        <v>4</v>
-      </c>
-      <c r="K21" t="n">
-        <v>2</v>
-      </c>
-      <c r="L21" t="n">
-        <v>3</v>
-      </c>
-      <c r="M21" t="n">
-        <v>1</v>
-      </c>
-      <c r="N21" t="n">
-        <v>39</v>
-      </c>
-      <c r="O21" t="n">
-        <v>59</v>
-      </c>
-      <c r="P21" t="n">
-        <v>3</v>
-      </c>
-      <c r="Q21" t="n">
-        <v>14</v>
-      </c>
-      <c r="R21" t="n">
-        <v>29</v>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="S21" t="inlineStr">
         <is>
@@ -3487,16 +3491,18 @@
       </c>
       <c r="T21" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="U21" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="V21" t="n">
-        <v>11</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="V21" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="W21" t="inlineStr">
         <is>
@@ -3525,7 +3531,7 @@
       </c>
       <c r="AB21" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="AC21" t="inlineStr">
@@ -3535,7 +3541,7 @@
       </c>
       <c r="AD21" t="inlineStr">
         <is>
-          <t>NOP</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="AE21" t="inlineStr">
@@ -3545,7 +3551,7 @@
       </c>
       <c r="AF21" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="AG21" t="inlineStr">
@@ -3555,7 +3561,7 @@
       </c>
       <c r="AH21" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="AI21" t="inlineStr">
@@ -3564,7 +3570,7 @@
         </is>
       </c>
       <c r="AJ21" t="n">
-        <v>-0.5</v>
+        <v>0.9</v>
       </c>
       <c r="AK21" t="inlineStr"/>
       <c r="AL21" t="inlineStr"/>
@@ -3572,12 +3578,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>NYK</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Bradley Beal</t>
+          <t>Donte DiVincenzo</t>
         </is>
       </c>
       <c r="C22" t="inlineStr"/>
@@ -3588,79 +3594,69 @@
       </c>
       <c r="E22" t="inlineStr"/>
       <c r="F22" t="n">
-        <v>26</v>
+        <v>21.8</v>
       </c>
       <c r="G22" t="n">
-        <v>26.9</v>
+        <v>26.3</v>
       </c>
       <c r="H22" t="n">
-        <v>26.2</v>
+        <v>18.5</v>
       </c>
       <c r="I22" t="n">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="J22" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="K22" t="n">
         <v>1</v>
       </c>
       <c r="L22" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N22" t="n">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="O22" t="n">
-        <v>10</v>
-      </c>
-      <c r="P22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="R22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>7</v>
+      </c>
+      <c r="P22" t="n">
+        <v>19</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>31</v>
+      </c>
+      <c r="R22" t="n">
+        <v>13</v>
       </c>
       <c r="S22" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T22" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="U22" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="V22" t="n">
+        <v>7</v>
       </c>
       <c r="W22" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X22" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="X22" t="n">
+        <v>22</v>
       </c>
       <c r="Y22" t="inlineStr">
         <is>
@@ -3679,7 +3675,7 @@
       </c>
       <c r="AB22" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>ORL</t>
         </is>
       </c>
       <c r="AC22" t="inlineStr">
@@ -3689,17 +3685,17 @@
       </c>
       <c r="AD22" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="AE22" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF22" t="inlineStr">
         <is>
-          <t>CLE</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="AG22" t="inlineStr">
@@ -3709,16 +3705,16 @@
       </c>
       <c r="AH22" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="AI22" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ22" t="n">
-        <v>0.9</v>
+        <v>-1</v>
       </c>
       <c r="AK22" t="inlineStr"/>
       <c r="AL22" t="inlineStr"/>
@@ -3726,56 +3722,58 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>NYK</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Donte DiVincenzo</t>
+          <t>Brandon Miller</t>
         </is>
       </c>
       <c r="C23" t="inlineStr"/>
       <c r="D23" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>F</t>
         </is>
       </c>
       <c r="E23" t="inlineStr"/>
       <c r="F23" t="n">
-        <v>21.8</v>
+        <v>19.6</v>
       </c>
       <c r="G23" t="n">
-        <v>26.3</v>
+        <v>26.1</v>
       </c>
       <c r="H23" t="n">
-        <v>18.5</v>
+        <v>21.1</v>
       </c>
       <c r="I23" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J23" t="n">
         <v>5</v>
       </c>
       <c r="K23" t="n">
+        <v>3</v>
+      </c>
+      <c r="L23" t="n">
+        <v>3</v>
+      </c>
+      <c r="M23" t="n">
         <v>1</v>
       </c>
-      <c r="L23" t="n">
-        <v>2</v>
-      </c>
-      <c r="M23" t="n">
-        <v>2</v>
-      </c>
       <c r="N23" t="n">
-        <v>39</v>
-      </c>
-      <c r="O23" t="n">
-        <v>7</v>
+        <v>38</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="P23" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="Q23" t="n">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="R23" t="n">
         <v>13</v>
@@ -3787,7 +3785,7 @@
       </c>
       <c r="T23" t="inlineStr">
         <is>
-          <t>ATL</t>
+          <t>ORL</t>
         </is>
       </c>
       <c r="U23" t="inlineStr">
@@ -3796,15 +3794,17 @@
         </is>
       </c>
       <c r="V23" t="n">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="W23" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="X23" t="n">
-        <v>22</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="X23" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Y23" t="inlineStr">
         <is>
@@ -3818,12 +3818,12 @@
       </c>
       <c r="AA23" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AB23" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="AC23" t="inlineStr">
@@ -3833,17 +3833,17 @@
       </c>
       <c r="AD23" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="AE23" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF23" t="inlineStr">
         <is>
-          <t>PHI</t>
+          <t>DET</t>
         </is>
       </c>
       <c r="AG23" t="inlineStr">
@@ -3853,7 +3853,7 @@
       </c>
       <c r="AH23" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AI23" t="inlineStr">
@@ -3862,7 +3862,7 @@
         </is>
       </c>
       <c r="AJ23" t="n">
-        <v>-1</v>
+        <v>1.7</v>
       </c>
       <c r="AK23" t="inlineStr"/>
       <c r="AL23" t="inlineStr"/>
@@ -3870,12 +3870,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CHA</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Brandon Miller</t>
+          <t>Michael Porter Jr.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr"/>
@@ -3886,45 +3886,43 @@
       </c>
       <c r="E24" t="inlineStr"/>
       <c r="F24" t="n">
-        <v>19.6</v>
+        <v>37.4</v>
       </c>
       <c r="G24" t="n">
         <v>26.1</v>
       </c>
       <c r="H24" t="n">
-        <v>21.1</v>
+        <v>24.2</v>
       </c>
       <c r="I24" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="J24" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="M24" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="N24" t="n">
-        <v>38</v>
-      </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>55</v>
+      </c>
+      <c r="O24" t="n">
+        <v>47</v>
       </c>
       <c r="P24" t="n">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="Q24" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="R24" t="n">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="S24" t="inlineStr">
         <is>
@@ -3933,7 +3931,7 @@
       </c>
       <c r="T24" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="U24" t="inlineStr">
@@ -3942,7 +3940,7 @@
         </is>
       </c>
       <c r="V24" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W24" t="inlineStr">
         <is>
@@ -3966,12 +3964,12 @@
       </c>
       <c r="AA24" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AB24" t="inlineStr">
         <is>
-          <t>WAS</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="AC24" t="inlineStr">
@@ -3981,17 +3979,17 @@
       </c>
       <c r="AD24" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>UTA</t>
         </is>
       </c>
       <c r="AE24" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF24" t="inlineStr">
         <is>
-          <t>DET</t>
+          <t>TOR</t>
         </is>
       </c>
       <c r="AG24" t="inlineStr">
@@ -4001,7 +3999,7 @@
       </c>
       <c r="AH24" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>MIA</t>
         </is>
       </c>
       <c r="AI24" t="inlineStr">
@@ -4018,77 +4016,77 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>DEN</t>
+          <t>IND</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Michael Porter Jr.</t>
+          <t>Tyrese Haliburton</t>
         </is>
       </c>
       <c r="C25" t="inlineStr"/>
       <c r="D25" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>G</t>
         </is>
       </c>
       <c r="E25" t="inlineStr"/>
       <c r="F25" t="n">
-        <v>37.4</v>
+        <v>15.6</v>
       </c>
       <c r="G25" t="n">
-        <v>26.1</v>
+        <v>23</v>
       </c>
       <c r="H25" t="n">
-        <v>24.2</v>
+        <v>35.3</v>
       </c>
       <c r="I25" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J25" t="n">
         <v>4</v>
       </c>
       <c r="K25" t="n">
+        <v>2</v>
+      </c>
+      <c r="L25" t="n">
+        <v>4</v>
+      </c>
+      <c r="M25" t="n">
         <v>1</v>
       </c>
-      <c r="L25" t="n">
-        <v>1</v>
-      </c>
-      <c r="M25" t="n">
-        <v>4</v>
-      </c>
       <c r="N25" t="n">
-        <v>55</v>
+        <v>16</v>
       </c>
       <c r="O25" t="n">
-        <v>47</v>
+        <v>-8</v>
       </c>
       <c r="P25" t="n">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="Q25" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="R25" t="n">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="S25" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="T25" t="inlineStr">
         <is>
-          <t>PHX</t>
+          <t>DAL</t>
         </is>
       </c>
       <c r="U25" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="V25" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="W25" t="inlineStr">
         <is>
@@ -4117,42 +4115,42 @@
       </c>
       <c r="AB25" t="inlineStr">
         <is>
-          <t>BOS</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AC25" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AD25" t="inlineStr">
         <is>
-          <t>UTA</t>
+          <t>ORL</t>
         </is>
       </c>
       <c r="AE25" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AF25" t="inlineStr">
         <is>
-          <t>TOR</t>
+          <t>OKC</t>
         </is>
       </c>
       <c r="AG25" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AH25" t="inlineStr">
         <is>
-          <t>MIA</t>
+          <t>CHI</t>
         </is>
       </c>
       <c r="AI25" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AJ25" t="n">
@@ -4164,12 +4162,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>HOU</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Tyrese Haliburton</t>
+          <t>Fred VanVleet</t>
         </is>
       </c>
       <c r="C26" t="inlineStr"/>
@@ -4180,52 +4178,52 @@
       </c>
       <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
-        <v>15.6</v>
+        <v>24.6</v>
       </c>
       <c r="G26" t="n">
-        <v>23</v>
+        <v>22.5</v>
       </c>
       <c r="H26" t="n">
-        <v>35.3</v>
+        <v>26.2</v>
       </c>
       <c r="I26" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="J26" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K26" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" t="n">
         <v>2</v>
-      </c>
-      <c r="L26" t="n">
-        <v>5</v>
       </c>
       <c r="M26" t="n">
         <v>1</v>
       </c>
       <c r="N26" t="n">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="O26" t="n">
-        <v>-8</v>
+        <v>30</v>
       </c>
       <c r="P26" t="n">
-        <v>31</v>
+        <v>-2</v>
       </c>
       <c r="Q26" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="R26" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S26" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="T26" t="inlineStr">
         <is>
-          <t>DAL</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="U26" t="inlineStr">
@@ -4234,17 +4232,15 @@
         </is>
       </c>
       <c r="V26" t="n">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="W26" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X26" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="X26" t="n">
+        <v>36</v>
       </c>
       <c r="Y26" t="inlineStr">
         <is>
@@ -4263,7 +4259,7 @@
       </c>
       <c r="AB26" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>LAC</t>
         </is>
       </c>
       <c r="AC26" t="inlineStr">
@@ -4273,7 +4269,7 @@
       </c>
       <c r="AD26" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="AE26" t="inlineStr">
@@ -4283,26 +4279,26 @@
       </c>
       <c r="AF26" t="inlineStr">
         <is>
-          <t>OKC</t>
+          <t>SAC</t>
         </is>
       </c>
       <c r="AG26" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AH26" t="inlineStr">
         <is>
-          <t>CHI</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="AI26" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AJ26" t="n">
-        <v>1.7</v>
+        <v>-0.7</v>
       </c>
       <c r="AK26" t="inlineStr"/>
       <c r="AL26" t="inlineStr"/>
@@ -4310,15 +4306,19 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>HOU</t>
+          <t>CLE</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Fred VanVleet</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr"/>
+          <t>Donovan Mitchell</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
       <c r="D27" t="inlineStr">
         <is>
           <t>G</t>
@@ -4326,43 +4326,47 @@
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="n">
-        <v>24.6</v>
+        <v>38.4</v>
       </c>
       <c r="G27" t="n">
-        <v>22.5</v>
+        <v>41.1</v>
       </c>
       <c r="H27" t="n">
-        <v>26.2</v>
+        <v>39.9</v>
       </c>
       <c r="I27" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="J27" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" t="n">
         <v>3</v>
       </c>
-      <c r="K27" t="n">
-        <v>1</v>
-      </c>
       <c r="L27" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M27" t="n">
-        <v>1</v>
-      </c>
-      <c r="N27" t="n">
-        <v>42</v>
-      </c>
-      <c r="O27" t="n">
-        <v>30</v>
+        <v>6</v>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="P27" t="n">
-        <v>-2</v>
+        <v>21</v>
       </c>
       <c r="Q27" t="n">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="R27" t="n">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="S27" t="inlineStr">
         <is>
@@ -4371,16 +4375,16 @@
       </c>
       <c r="T27" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>BOS</t>
         </is>
       </c>
       <c r="U27" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="V27" t="n">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="W27" t="inlineStr">
         <is>
@@ -4388,7 +4392,7 @@
         </is>
       </c>
       <c r="X27" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Y27" t="inlineStr">
         <is>
@@ -4402,42 +4406,42 @@
       </c>
       <c r="AA27" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AB27" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="AC27" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AD27" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AE27" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AF27" t="inlineStr">
         <is>
-          <t>SAC</t>
+          <t>BKN</t>
         </is>
       </c>
       <c r="AG27" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AH27" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>PHX</t>
         </is>
       </c>
       <c r="AI27" t="inlineStr">
@@ -4446,7 +4450,7 @@
         </is>
       </c>
       <c r="AJ27" t="n">
-        <v>-0.7</v>
+        <v>4</v>
       </c>
       <c r="AK27" t="inlineStr"/>
       <c r="AL27" t="inlineStr"/>
@@ -4483,13 +4487,13 @@
         <v>41.4</v>
       </c>
       <c r="I28" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J28" t="n">
         <v>1</v>
       </c>
       <c r="K28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" t="n">
         <v>4</v>

</xml_diff>